<commit_message>
v16.4 engine update - PPE normaliser added
</commit_message>
<xml_diff>
--- a/rpd-v8-upgrade/phase-2-whsmp-update/swms/RPD_SWMS_Consolidation_Traceability_Map_1.xlsx
+++ b/rpd-v8-upgrade/phase-2-whsmp-update/swms/RPD_SWMS_Consolidation_Traceability_Map_1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlanRichardson\gatekeeper\rpd-v8-upgrade\phase-2-whsmp-update\swms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B1A9949-015E-4A68-9EE0-012C4C15B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB388C3-81F9-4696-B775-7FF4632DCF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30030" yWindow="-3645" windowWidth="17910" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30435" yWindow="-3645" windowWidth="20070" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Traceability Map" sheetId="1" r:id="rId1"/>
-    <sheet name="New SWMS Structure" sheetId="2" r:id="rId2"/>
+    <sheet name="New SWMS Structure" sheetId="2" r:id="rId1"/>
+    <sheet name="Traceability Map" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'New SWMS Structure'!$A$1:$E$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'New SWMS Structure'!$A$1:$E$25</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -29,9 +29,6 @@
     <t>RPD SWMS CONSOLIDATION — TRACEABILITY MAP</t>
   </si>
   <si>
-    <t>Purpose: Trace every existing SWI and SWMS to its destination in the new structure. Ensures nothing is lost and RPD can demonstrate change management to auditors.</t>
-  </si>
-  <si>
     <t>INTEGRATED = content absorbed into a Master SWMS  |  LINE ITEM = high-risk activity added as line item in Master  |  STANDALONE SWMS = remains separate  |  SUPERSEDED = replaced, content covered elsewhere</t>
   </si>
   <si>
@@ -609,13 +606,16 @@
   </si>
   <si>
     <t>46 documents (34 SWMS + 12 SWIs)</t>
+  </si>
+  <si>
+    <t>Trace every existing SWI and SWMS to its destination in the new structure. Ensures nothing is lost and RPD can demonstrate change management.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,12 +640,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -661,6 +655,18 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -702,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -777,13 +783,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -797,9 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,13 +845,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,6 +1162,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="75" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1131,8 +1522,8 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H53"/>
+      <pane ySplit="6" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,103 +1539,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1252,25 +1643,25 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1278,22 +1669,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -1302,25 +1693,25 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1328,25 +1719,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1354,22 +1745,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -1378,25 +1769,25 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1404,25 +1795,25 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1430,25 +1821,25 @@
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1456,25 +1847,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="G16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1482,72 +1873,72 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>12</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
-        <v>12</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="G20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -1556,22 +1947,22 @@
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -1580,22 +1971,22 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -1604,22 +1995,22 @@
         <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="3"/>
     </row>
@@ -1628,25 +2019,25 @@
         <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1654,22 +2045,22 @@
         <v>18</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="G25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="3"/>
     </row>
@@ -1678,22 +2069,22 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -1702,22 +2093,22 @@
         <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3"/>
     </row>
@@ -1726,22 +2117,22 @@
         <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="G28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="3"/>
     </row>
@@ -1750,22 +2141,22 @@
         <v>22</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3"/>
     </row>
@@ -1774,22 +2165,22 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="G30" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -1798,25 +2189,25 @@
         <v>24</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1824,22 +2215,22 @@
         <v>25</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="G32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="3"/>
     </row>
@@ -1848,25 +2239,25 @@
         <v>26</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1874,22 +2265,22 @@
         <v>27</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="G34" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="3"/>
     </row>
@@ -1898,22 +2289,22 @@
         <v>28</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="G35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -1922,25 +2313,25 @@
         <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="G36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1948,22 +2339,22 @@
         <v>30</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="G37" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" s="3"/>
     </row>
@@ -1972,22 +2363,22 @@
         <v>31</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="G38" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -1996,22 +2387,22 @@
         <v>32</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="G39" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H39" s="3"/>
     </row>
@@ -2020,22 +2411,22 @@
         <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="G40" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" s="3"/>
     </row>
@@ -2044,22 +2435,22 @@
         <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="G41" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" s="3"/>
     </row>
@@ -2068,22 +2459,22 @@
         <v>35</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="G42" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H42" s="3"/>
     </row>
@@ -2092,25 +2483,25 @@
         <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="9" t="s">
+      <c r="E43" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H43" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2118,25 +2509,25 @@
         <v>37</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2144,22 +2535,22 @@
         <v>38</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="G45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" s="3"/>
     </row>
@@ -2168,22 +2559,22 @@
         <v>39</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="G46" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H46" s="3"/>
     </row>
@@ -2192,25 +2583,25 @@
         <v>40</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2218,25 +2609,25 @@
         <v>41</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>106</v>
+      <c r="G48" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2244,25 +2635,25 @@
         <v>42</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>106</v>
+      <c r="G49" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2270,25 +2661,25 @@
         <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>106</v>
+      <c r="G50" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2296,25 +2687,25 @@
         <v>44</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2322,25 +2713,25 @@
         <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>106</v>
+      <c r="G52" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2348,29 +2739,30 @@
         <v>46</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>106</v>
+      <c r="G53" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A2:H2"/>
@@ -2380,357 +2772,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="4" spans="1:5" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B25" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="85" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>